<commit_message>
Stabilizing and Tests 10, 17.
</commit_message>
<xml_diff>
--- a/Motorola Stability Tests.xlsx
+++ b/Motorola Stability Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="125">
   <si>
     <t>High</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>6-10-2013</t>
+  </si>
+  <si>
+    <t>Awaiting design from Brian + Roland</t>
+  </si>
+  <si>
+    <t>6-11-2013</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +448,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -529,6 +541,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3237,7 +3256,7 @@
   <dimension ref="A1:L84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,14 +3315,14 @@
         <v>26</v>
       </c>
       <c r="J3" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="9">
         <f>J3/I3</f>
-        <v>0.46153846153846156</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3400,14 +3419,14 @@
       </c>
       <c r="J6" s="5">
         <f>SUM(J3:J5)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="0"/>
-        <v>0.56896551724137934</v>
+        <v>0.60344827586206895</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3453,20 +3472,24 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="13">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="13">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3504,20 +3527,24 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="13">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3555,20 +3582,20 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="19">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="2" t="s">
+      <c r="C15" s="19">
+        <v>3</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -3576,20 +3603,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="19">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="2" t="s">
+      <c r="C16" s="19">
+        <v>3</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G16" s="8" t="s">
@@ -3597,20 +3624,20 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="19">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="19">
+        <v>3</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -3618,20 +3645,20 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="19">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="2" t="s">
+      <c r="C18" s="19">
+        <v>3</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -3771,38 +3798,46 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="19">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="2">
-        <v>3</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="8"/>
+      <c r="C25" s="19">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="19">
         <v>66</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="2">
-        <v>3</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="8"/>
+      <c r="C26" s="19">
+        <v>3</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
@@ -4096,20 +4131,20 @@
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="19">
         <v>46</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="s">
+      <c r="C42" s="19">
+        <v>2</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G42" s="8" t="s">
@@ -4117,20 +4152,20 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="19">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="2">
-        <v>2</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2" t="s">
+      <c r="C43" s="19">
+        <v>2</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G43" s="8" t="s">

</xml_diff>

<commit_message>
Stabilizing and Tests 11, 12, 13, 18, 19.
</commit_message>
<xml_diff>
--- a/Motorola Stability Tests.xlsx
+++ b/Motorola Stability Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="127">
   <si>
     <t>High</t>
   </si>
@@ -360,9 +360,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve">  Uses browser to visit Top 5 websites by traffic.</t>
-  </si>
-  <si>
     <t>Coverage obtained via test 35.</t>
   </si>
   <si>
@@ -396,10 +393,19 @@
     <t>6-10-2013</t>
   </si>
   <si>
-    <t>Awaiting design from Brian + Roland</t>
-  </si>
-  <si>
     <t>6-11-2013</t>
+  </si>
+  <si>
+    <t>6-12-2012</t>
+  </si>
+  <si>
+    <t>6-12-2013</t>
+  </si>
+  <si>
+    <t>6-13-2013</t>
+  </si>
+  <si>
+    <t>Uses browser to visit Top 5 websites by traffic.</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -548,6 +554,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,7 +1133,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -2303,7 +2313,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -3315,14 +3325,14 @@
         <v>26</v>
       </c>
       <c r="J3" s="4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="9">
         <f>J3/I3</f>
-        <v>0.53846153846153844</v>
+        <v>0.69230769230769229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3339,24 +3349,24 @@
         <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G4" s="8"/>
       <c r="I4" s="4">
         <v>21</v>
       </c>
       <c r="J4" s="4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" ref="L4:L6" si="0">J4/I4</f>
-        <v>0.5714285714285714</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3373,10 +3383,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="4">
@@ -3407,10 +3417,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6" s="8"/>
       <c r="I6" s="5">
@@ -3419,14 +3429,14 @@
       </c>
       <c r="J6" s="5">
         <f>SUM(J3:J5)</f>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="0"/>
-        <v>0.60344827586206895</v>
+        <v>0.75862068965517238</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3443,10 +3453,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -3464,10 +3474,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -3485,45 +3495,53 @@
         <v>0</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="13">
+        <v>3</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="13">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="13">
+        <v>3</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3540,45 +3558,53 @@
         <v>0</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="13">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="13">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3596,10 +3622,10 @@
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3617,10 +3643,10 @@
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3638,10 +3664,10 @@
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3659,10 +3685,10 @@
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,10 +3705,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" s="8"/>
     </row>
@@ -3700,10 +3726,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G20" s="8"/>
     </row>
@@ -3721,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="8"/>
     </row>
@@ -3745,7 +3771,7 @@
         <v>101</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>105</v>
@@ -3768,7 +3794,7 @@
         <v>101</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>104</v>
@@ -3791,53 +3817,45 @@
         <v>101</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="22">
         <v>65</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="19">
-        <v>3</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="C25" s="22">
+        <v>3</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="22">
         <v>66</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="19">
-        <v>3</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="C26" s="22">
+        <v>3</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
@@ -3856,10 +3874,10 @@
         <v>109</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,7 +3931,7 @@
         <v>101</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G30" s="8"/>
     </row>
@@ -3934,93 +3952,113 @@
         <v>101</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="13">
         <v>11</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="2">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="C32" s="13">
+        <v>2</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="13">
         <v>12</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="2">
-        <v>2</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="C33" s="13">
+        <v>2</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="13">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="2">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="C34" s="13">
+        <v>2</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="13">
         <v>15</v>
       </c>
-      <c r="B35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="2">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="B35" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="13">
+        <v>2</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="13">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="2">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="C36" s="13">
+        <v>2</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4040,10 +4078,10 @@
         <v>101</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4063,7 +4101,7 @@
         <v>101</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G38" s="8"/>
     </row>
@@ -4084,7 +4122,7 @@
         <v>98</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G39" s="8"/>
     </row>
@@ -4105,7 +4143,7 @@
         <v>101</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G40" s="8"/>
     </row>
@@ -4126,7 +4164,7 @@
         <v>98</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G41" s="8"/>
     </row>
@@ -4145,10 +4183,10 @@
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4166,10 +4204,10 @@
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -4189,7 +4227,7 @@
         <v>109</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G44" s="8"/>
     </row>
@@ -4210,7 +4248,7 @@
         <v>97</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G45" s="8"/>
     </row>
@@ -4231,7 +4269,7 @@
         <v>97</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>99</v>
@@ -4254,7 +4292,7 @@
         <v>97</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>100</v>
@@ -4277,7 +4315,7 @@
         <v>107</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G48" s="8"/>
     </row>
@@ -4332,7 +4370,7 @@
         <v>106</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G51" s="8"/>
     </row>
@@ -4353,7 +4391,7 @@
         <v>107</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G52" s="8"/>
     </row>
@@ -4374,7 +4412,7 @@
         <v>109</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G53" s="8"/>
     </row>
@@ -4395,7 +4433,7 @@
         <v>109</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G54" s="8"/>
     </row>
@@ -4416,7 +4454,7 @@
         <v>109</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G55" s="8"/>
     </row>
@@ -4440,7 +4478,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -4463,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -4486,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -4509,7 +4547,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -4529,7 +4567,7 @@
         <v>106</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G60" s="8"/>
     </row>
@@ -4550,7 +4588,7 @@
         <v>106</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G61" s="8"/>
     </row>
@@ -4571,7 +4609,7 @@
         <v>106</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G62" s="8"/>
     </row>
@@ -4592,7 +4630,7 @@
         <v>107</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G63" s="8"/>
     </row>
@@ -4650,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -4673,7 +4711,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -4696,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -4719,7 +4757,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -4742,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -4765,7 +4803,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4788,7 +4826,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4811,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4831,7 +4869,7 @@
         <v>93</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G74" s="8"/>
     </row>
@@ -4852,7 +4890,7 @@
         <v>93</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G75" s="8"/>
     </row>
@@ -4873,7 +4911,7 @@
         <v>93</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G76" s="8"/>
     </row>
@@ -4894,7 +4932,7 @@
         <v>93</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G77" s="8"/>
     </row>
@@ -4915,7 +4953,7 @@
         <v>93</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G78" s="8"/>
     </row>
@@ -4936,7 +4974,7 @@
         <v>93</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G79" s="8"/>
     </row>
@@ -4957,7 +4995,7 @@
         <v>93</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G80" s="8"/>
     </row>
@@ -4978,7 +5016,7 @@
         <v>93</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G81" s="8"/>
     </row>
@@ -4999,7 +5037,7 @@
         <v>93</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G82" s="8"/>
     </row>
@@ -5020,7 +5058,7 @@
         <v>93</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G83" s="8"/>
     </row>
@@ -5041,7 +5079,7 @@
         <v>93</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G84" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updates for Shelter build 1.25.
</commit_message>
<xml_diff>
--- a/Motorola Stability Tests.xlsx
+++ b/Motorola Stability Tests.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Master Test List" sheetId="1" r:id="rId1"/>
     <sheet name="Sortable List" sheetId="2" r:id="rId2"/>
     <sheet name="Completed Items" sheetId="3" r:id="rId3"/>
+    <sheet name="Eggplant Scripts" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Completed Items'!$A$3:$G$3</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="159">
   <si>
     <t>High</t>
   </si>
@@ -406,6 +407,102 @@
   </si>
   <si>
     <t>Uses browser to visit Top 5 websites by traffic.</t>
+  </si>
+  <si>
+    <t>Eggplant Scripts</t>
+  </si>
+  <si>
+    <t>09+08</t>
+  </si>
+  <si>
+    <t>Tests covered</t>
+  </si>
+  <si>
+    <t>Test functions</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Exe Time</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>30+33+35</t>
+  </si>
+  <si>
+    <t>Apps</t>
+  </si>
+  <si>
+    <t>37+39</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>38+40</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>44+45+46</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>47+48+49</t>
+  </si>
+  <si>
+    <t>Rec Audio</t>
+  </si>
+  <si>
+    <t>Rec Video</t>
+  </si>
+  <si>
+    <t>Rec Image</t>
+  </si>
+  <si>
+    <t>50+51+52</t>
+  </si>
+  <si>
+    <t>Video Stream</t>
+  </si>
+  <si>
+    <t>54+55+56</t>
+  </si>
+  <si>
+    <t>Play Music</t>
+  </si>
+  <si>
+    <t>Set wallpaper</t>
+  </si>
+  <si>
+    <t>61+26+24+25+62+63</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>65+66</t>
+  </si>
+  <si>
+    <t>Menu Nav</t>
+  </si>
+  <si>
+    <t>WiFi</t>
+  </si>
+  <si>
+    <t>NFC</t>
+  </si>
+  <si>
+    <t>Schedules</t>
+  </si>
+  <si>
+    <t>2G Call</t>
   </si>
 </sst>
 </file>
@@ -501,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -558,6 +655,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2081,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5093,4 +5199,340 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="25">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.10902777777777778</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="25">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="25">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="25">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>53</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.1361111111111111</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="25">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="25">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="25">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>64</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="25">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="25">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="26">
+        <f>SUM(C3:C16)</f>
+        <v>0.92638888888888882</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final scriptable testcases and polishing.
</commit_message>
<xml_diff>
--- a/Motorola Stability Tests.xlsx
+++ b/Motorola Stability Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-5955" yWindow="360" windowWidth="24000" windowHeight="10110" activeTab="2"/>
+    <workbookView xWindow="-5955" yWindow="360" windowWidth="24000" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Master Test List" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="180">
   <si>
     <t>High</t>
   </si>
@@ -503,12 +503,78 @@
   </si>
   <si>
     <t>2G Call</t>
+  </si>
+  <si>
+    <t>3G Call</t>
+  </si>
+  <si>
+    <t>2G Call from History</t>
+  </si>
+  <si>
+    <t>3G Call from History</t>
+  </si>
+  <si>
+    <t>SMS Max Chars</t>
+  </si>
+  <si>
+    <t>MMS Audio</t>
+  </si>
+  <si>
+    <t>MMS Video</t>
+  </si>
+  <si>
+    <t>MMS Image</t>
+  </si>
+  <si>
+    <t>Email no attach</t>
+  </si>
+  <si>
+    <t>Email with attach</t>
+  </si>
+  <si>
+    <t>Phone Dial</t>
+  </si>
+  <si>
+    <t>6-25-2013</t>
+  </si>
+  <si>
+    <t>Requires USB set up.</t>
+  </si>
+  <si>
+    <t>6-26-2013</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>Hotspot</t>
+  </si>
+  <si>
+    <t>Tether</t>
+  </si>
+  <si>
+    <t>Awaiting device bug fix OR clarification from Motorola.</t>
+  </si>
+  <si>
+    <t>Awaiting clarification from Motorola.</t>
+  </si>
+  <si>
+    <t>Awaiting bug fixes</t>
+  </si>
+  <si>
+    <t>Awaiting fixes or clarication</t>
+  </si>
+  <si>
+    <t>Awaiting clarification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[m]:ss"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -643,7 +709,6 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,18 +716,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2187,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3431,14 +3502,14 @@
         <v>26</v>
       </c>
       <c r="J3" s="4">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="9">
         <f>J3/I3</f>
-        <v>0.69230769230769229</v>
+        <v>0.84615384615384615</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3535,14 +3606,14 @@
       </c>
       <c r="J6" s="5">
         <f>SUM(J3:J5)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="0"/>
-        <v>0.75862068965517238</v>
+        <v>0.82758620689655171</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3586,6 +3657,12 @@
         <v>116</v>
       </c>
       <c r="G8" s="8"/>
+      <c r="J8" s="26">
+        <v>6</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
@@ -3607,6 +3684,12 @@
         <v>116</v>
       </c>
       <c r="G9" s="8"/>
+      <c r="J9" s="26">
+        <v>2</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
@@ -3628,6 +3711,12 @@
         <v>116</v>
       </c>
       <c r="G10" s="8"/>
+      <c r="J10" s="26">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
@@ -3714,20 +3803,20 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>44</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="19">
-        <v>3</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19" t="s">
+      <c r="C15" s="18">
+        <v>3</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -3735,20 +3824,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>45</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="19">
-        <v>3</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="19" t="s">
+      <c r="C16" s="18">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G16" s="8" t="s">
@@ -3756,20 +3845,20 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>47</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="19">
-        <v>3</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="19" t="s">
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -3777,20 +3866,20 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>48</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="19">
-        <v>3</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19" t="s">
+      <c r="C18" s="18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -3930,38 +4019,50 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="13">
         <v>65</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="22">
-        <v>3</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="8"/>
+      <c r="C25" s="13">
+        <v>3</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="13">
         <v>66</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="22">
-        <v>3</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="8"/>
+      <c r="C26" s="13">
+        <v>3</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
@@ -3987,37 +4088,45 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="13">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="2">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="13">
+        <v>3</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="13">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="2">
-        <v>3</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="13">
+        <v>3</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4275,20 +4384,20 @@
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
+      <c r="A42" s="18">
         <v>46</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="19">
-        <v>2</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="18">
+        <v>2</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G42" s="8" t="s">
@@ -4296,20 +4405,20 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
+      <c r="A43" s="18">
         <v>49</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="19">
-        <v>2</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19" t="s">
+      <c r="C43" s="18">
+        <v>2</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G43" s="8" t="s">
@@ -4426,38 +4535,46 @@
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
+      <c r="A49" s="24">
         <v>69</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="10">
-        <v>2</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E49" s="10"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="8"/>
+      <c r="C49" s="24">
+        <v>2</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
+      <c r="A50" s="24">
         <v>72</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="10">
-        <v>2</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="10"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="8"/>
+      <c r="C50" s="24">
+        <v>2</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="24"/>
+      <c r="F50" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
@@ -4741,38 +4858,42 @@
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="10">
+      <c r="A64" s="24">
         <v>68</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="10">
-        <v>1</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="8"/>
+      <c r="C64" s="24">
+        <v>1</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="24"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="8" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="10">
+      <c r="A65" s="24">
         <v>71</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="10">
-        <v>1</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" s="10"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="8"/>
+      <c r="C65" s="24">
+        <v>1</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="24"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="8" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
@@ -5203,16 +5324,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5221,13 +5343,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -5241,8 +5363,8 @@
       <c r="B3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="25">
-        <v>5.7638888888888885E-2</v>
+      <c r="C3" s="22">
+        <v>1.25E-3</v>
       </c>
       <c r="D3" s="2">
         <v>1.25</v>
@@ -5255,8 +5377,8 @@
       <c r="B4" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="25">
-        <v>0.10902777777777778</v>
+      <c r="C4" s="22">
+        <v>2.0949074074074073E-3</v>
       </c>
       <c r="D4" s="2">
         <v>1.25</v>
@@ -5269,8 +5391,8 @@
       <c r="B5" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="25">
-        <v>4.7222222222222221E-2</v>
+      <c r="C5" s="22">
+        <v>1.1574074074074073E-3</v>
       </c>
       <c r="D5" s="2">
         <v>1.25</v>
@@ -5283,8 +5405,8 @@
       <c r="B6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="25">
-        <v>4.2361111111111106E-2</v>
+      <c r="C6" s="22">
+        <v>7.5231481481481471E-4</v>
       </c>
       <c r="D6" s="2">
         <v>1.25</v>
@@ -5297,8 +5419,8 @@
       <c r="B7" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="25">
-        <v>4.1666666666666664E-2</v>
+      <c r="C7" s="22">
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>141</v>
@@ -5311,8 +5433,8 @@
       <c r="B8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="25">
-        <v>4.1666666666666664E-2</v>
+      <c r="C8" s="22">
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>141</v>
@@ -5325,8 +5447,8 @@
       <c r="B9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="25">
-        <v>3.125E-2</v>
+      <c r="C9" s="22">
+        <v>9.7222222222222209E-4</v>
       </c>
       <c r="D9" s="2">
         <v>1.25</v>
@@ -5339,8 +5461,8 @@
       <c r="B10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="25">
-        <v>0.1361111111111111</v>
+      <c r="C10" s="22">
+        <v>2.3842592592592591E-3</v>
       </c>
       <c r="D10" s="2">
         <v>1.25</v>
@@ -5353,8 +5475,8 @@
       <c r="B11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="25">
-        <v>6.5972222222222224E-2</v>
+      <c r="C11" s="22">
+        <v>1.2962962962962963E-3</v>
       </c>
       <c r="D11" s="2">
         <v>1.25</v>
@@ -5367,8 +5489,8 @@
       <c r="B12" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="25">
-        <v>5.9722222222222225E-2</v>
+      <c r="C12" s="22">
+        <v>9.6064814814814808E-4</v>
       </c>
       <c r="D12" s="2">
         <v>1.25</v>
@@ -5381,8 +5503,8 @@
       <c r="B13" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="25">
-        <v>0.13541666666666666</v>
+      <c r="C13" s="22">
+        <v>2.8472222222222219E-3</v>
       </c>
       <c r="D13" s="2">
         <v>1.25</v>
@@ -5395,8 +5517,8 @@
       <c r="B14" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="25">
-        <v>6.1111111111111116E-2</v>
+      <c r="C14" s="22">
+        <v>1.2731481481481483E-3</v>
       </c>
       <c r="D14" s="2">
         <v>1.25</v>
@@ -5409,11 +5531,11 @@
       <c r="B15" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C15" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>141</v>
+      <c r="C15" s="22">
+        <v>5.7291666666666671E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5423,49 +5545,49 @@
       <c r="B16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="25">
-        <v>5.5555555555555552E-2</v>
+      <c r="C16" s="22">
+        <v>1.25E-3</v>
       </c>
       <c r="D16" s="2">
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="26">
+      <c r="C17" s="23">
         <f>SUM(C3:C16)</f>
-        <v>0.92638888888888882</v>
+        <v>2.3356481481481485E-2</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>0</v>
       </c>
@@ -5473,63 +5595,217 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="C22" s="22">
+        <v>1.7013888888888892E-3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="22">
+        <v>7.8703703703703705E-4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1.9791666666666668E-3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1.0300925925925926E-3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="22">
+        <v>9.4907407407407408E-4</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1.4814814814814814E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>12</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1.4583333333333334E-3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1.2152777777777778E-3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>18</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1.2384259259259258E-3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="22">
+        <v>2.5115740740740741E-3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>58</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="22">
+        <v>1.25E-3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>68</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="22">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="22">
+        <v>6.6203703703703702E-3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>70</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="22">
+        <v>6.4814814814814813E-3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="23">
+        <f>SUM(C22:C35)</f>
+        <v>2.9398148148148145E-2</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="G36" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates for Shelter build 1.29.
</commit_message>
<xml_diff>
--- a/Motorola Stability Tests.xlsx
+++ b/Motorola Stability Tests.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="178">
   <si>
     <t>High</t>
   </si>
@@ -553,19 +553,13 @@
     <t>Tether</t>
   </si>
   <si>
-    <t>Awaiting device bug fix OR clarification from Motorola.</t>
-  </si>
-  <si>
-    <t>Awaiting clarification from Motorola.</t>
-  </si>
-  <si>
     <t>Awaiting bug fixes</t>
   </si>
   <si>
-    <t>Awaiting fixes or clarication</t>
-  </si>
-  <si>
-    <t>Awaiting clarification</t>
+    <t>Awaiting Motorola/ProtoTest design analysis.</t>
+  </si>
+  <si>
+    <t>Awaiting design analysis</t>
   </si>
 </sst>
 </file>
@@ -3661,7 +3655,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3685,10 +3679,10 @@
       </c>
       <c r="G9" s="8"/>
       <c r="J9" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3711,12 +3705,7 @@
         <v>116</v>
       </c>
       <c r="G10" s="8"/>
-      <c r="J10" s="26">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>179</v>
-      </c>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
@@ -4552,7 +4541,7 @@
         <v>118</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -4573,7 +4562,7 @@
         <v>118</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -4871,7 +4860,9 @@
         <v>3</v>
       </c>
       <c r="E64" s="24"/>
-      <c r="F64" s="18"/>
+      <c r="F64" s="18" t="s">
+        <v>118</v>
+      </c>
       <c r="G64" s="8" t="s">
         <v>176</v>
       </c>
@@ -4890,7 +4881,9 @@
         <v>3</v>
       </c>
       <c r="E65" s="24"/>
-      <c r="F65" s="18"/>
+      <c r="F65" s="18" t="s">
+        <v>118</v>
+      </c>
       <c r="G65" s="8" t="s">
         <v>176</v>
       </c>
@@ -5326,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,7 +5360,7 @@
         <v>1.25E-3</v>
       </c>
       <c r="D3" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5381,7 +5374,7 @@
         <v>2.0949074074074073E-3</v>
       </c>
       <c r="D4" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5395,7 +5388,7 @@
         <v>1.1574074074074073E-3</v>
       </c>
       <c r="D5" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5409,7 +5402,7 @@
         <v>7.5231481481481471E-4</v>
       </c>
       <c r="D6" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5451,7 +5444,7 @@
         <v>9.7222222222222209E-4</v>
       </c>
       <c r="D9" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5465,7 +5458,7 @@
         <v>2.3842592592592591E-3</v>
       </c>
       <c r="D10" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5479,7 +5472,7 @@
         <v>1.2962962962962963E-3</v>
       </c>
       <c r="D11" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,7 +5486,7 @@
         <v>9.6064814814814808E-4</v>
       </c>
       <c r="D12" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,7 +5500,7 @@
         <v>2.8472222222222219E-3</v>
       </c>
       <c r="D13" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,7 +5514,7 @@
         <v>1.2731481481481483E-3</v>
       </c>
       <c r="D14" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,7 +5528,7 @@
         <v>5.7291666666666671E-3</v>
       </c>
       <c r="D15" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,7 +5542,7 @@
         <v>1.25E-3</v>
       </c>
       <c r="D16" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5606,7 +5599,7 @@
         <v>1.7013888888888892E-3</v>
       </c>
       <c r="D22" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5620,7 +5613,7 @@
         <v>7.8703703703703705E-4</v>
       </c>
       <c r="D23" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5634,7 +5627,7 @@
         <v>1.9791666666666668E-3</v>
       </c>
       <c r="D24" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5648,7 +5641,7 @@
         <v>1.0300925925925926E-3</v>
       </c>
       <c r="D25" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5662,7 +5655,7 @@
         <v>9.4907407407407408E-4</v>
       </c>
       <c r="D26" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5676,7 +5669,7 @@
         <v>1.4814814814814814E-3</v>
       </c>
       <c r="D27" s="2">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5779,8 +5772,8 @@
       <c r="C34" s="22">
         <v>6.6203703703703702E-3</v>
       </c>
-      <c r="D34" s="2">
-        <v>1.25</v>
+      <c r="D34" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="G34" s="22"/>
     </row>

</xml_diff>